<commit_message>
new beamraymar table in ruplin
</commit_message>
<xml_diff>
--- a/FileGunBasin/9 August-04 StormBasin/230 next push hurricane/230 next push hurricane 1.xlsx
+++ b/FileGunBasin/9 August-04 StormBasin/230 next push hurricane/230 next push hurricane 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylecampbell/Documents/repos/localrepo-snefuru4/FileGunBasin/9 August-04 StormBasin/230 next push hurricane/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808EEE00-F5EA-5F4E-A511-6C966F27EA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD53980-D9DF-734B-B4CC-29E7A7CDE695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19320" xr2:uid="{A19E904F-4B03-2145-9BA6-C366915416CF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="89">
   <si>
     <t>Elementor elicitor</t>
   </si>
@@ -300,6 +300,9 @@
   </si>
   <si>
     <t>_zen_orbitposts.hudson_imgplanbatch_id</t>
+  </si>
+  <si>
+    <t>79f1a2d4-ec7e-4f3a-a896-d2e4d0e2d3ba</t>
   </si>
 </sst>
 </file>
@@ -754,7 +757,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E140" sqref="E140"/>
+      <selection pane="bottomLeft" activeCell="E138" sqref="E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1094,6 +1097,11 @@
         <v>87</v>
       </c>
     </row>
+    <row r="149" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E149" t="s">
+        <v>88</v>
+      </c>
+    </row>
     <row r="156" spans="5:5" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="157" spans="5:5" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="161" spans="5:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
new toolbar column beamray
</commit_message>
<xml_diff>
--- a/FileGunBasin/9 August-04 StormBasin/230 next push hurricane/230 next push hurricane 1.xlsx
+++ b/FileGunBasin/9 August-04 StormBasin/230 next push hurricane/230 next push hurricane 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylecampbell/Documents/repos/localrepo-snefuru4/FileGunBasin/9 August-04 StormBasin/230 next push hurricane/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44DA162-1FA2-AF48-AC1D-E40DBA755303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85E4D55-3ED5-1C4F-BBF6-3E2C1ADDB1FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19320" xr2:uid="{A19E904F-4B03-2145-9BA6-C366915416CF}"/>
   </bookViews>
@@ -765,11 +765,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F70C95-EED0-8D44-855C-AAF817F310D3}">
-  <dimension ref="D1:H244"/>
+  <dimension ref="D1:H248"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E145" sqref="E145"/>
+      <selection pane="bottomLeft" activeCell="E146" sqref="E146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1130,162 +1130,150 @@
         <v>88</v>
       </c>
     </row>
-    <row r="156" spans="5:8" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="157" spans="5:8" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E161" s="5" t="s">
+    <row r="160" spans="5:8" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="161" spans="5:5" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="165" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E165" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E163" t="s">
+    <row r="167" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E167" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="168" spans="5:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="E168" s="9" t="s">
+    <row r="172" spans="5:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="E172" s="9" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E171" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E173" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="175" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E175" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E176" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="177" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E177" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="179" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E179" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="180" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E180" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="181" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E181" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="181" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E181" s="4" t="s">
+    <row r="185" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E185" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="182" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D182" s="6"/>
-      <c r="E182" s="6" t="s">
+    <row r="186" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D186" s="6"/>
+      <c r="E186" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="187" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E187" s="4" t="s">
+    <row r="191" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E191" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="188" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D188" s="6"/>
-      <c r="E188" s="6"/>
-    </row>
     <row r="192" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E192" s="4" t="s">
+      <c r="D192" s="6"/>
+      <c r="E192" s="6"/>
+    </row>
+    <row r="196" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E196" s="4" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="193" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D193" s="6"/>
-      <c r="E193" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="194" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D194" s="6"/>
-      <c r="E194" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="195" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D195" s="6"/>
-      <c r="E195" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="196" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D196" s="6"/>
-      <c r="E196" s="6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="197" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D197" s="6"/>
-      <c r="E197" s="6"/>
+      <c r="E197" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="198" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D198" s="6"/>
+      <c r="E198" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="199" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D199" s="6"/>
+      <c r="E199" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="200" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D200" s="6"/>
+      <c r="E200" s="6" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="201" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E201" s="4" t="s">
+      <c r="D201" s="6"/>
+      <c r="E201" s="6"/>
+    </row>
+    <row r="205" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E205" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="202" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D202" s="6"/>
-      <c r="E202" s="6" t="s">
+    <row r="206" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D206" s="6"/>
+      <c r="E206" s="6" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="206" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E206" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="207" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E207" s="4"/>
-    </row>
-    <row r="208" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D208" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E208" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="209" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E209" s="4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="210" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E210" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="211" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E211" s="4"/>
+    </row>
+    <row r="212" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D212" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E212" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="213" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E213" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="214" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E214" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="211" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D211" s="8" t="s">
+    <row r="215" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D215" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E211" s="4" t="s">
+      <c r="E215" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="212" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E212" s="4" t="s">
+    <row r="216" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E216" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="213" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D213" s="6"/>
-    </row>
-    <row r="214" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D214" s="6"/>
-    </row>
-    <row r="215" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D215" s="6"/>
-    </row>
-    <row r="216" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D216" s="6"/>
     </row>
     <row r="217" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D217" s="6"/>
@@ -1299,53 +1287,65 @@
     <row r="220" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D220" s="6"/>
     </row>
-    <row r="226" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E226" s="4" t="s">
+    <row r="221" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D221" s="6"/>
+    </row>
+    <row r="222" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D222" s="6"/>
+    </row>
+    <row r="223" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D223" s="6"/>
+    </row>
+    <row r="224" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D224" s="6"/>
+    </row>
+    <row r="230" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E230" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="227" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D227" s="6"/>
-      <c r="E227" s="4"/>
-    </row>
-    <row r="228" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D228" s="6"/>
-      <c r="E228" s="4"/>
-    </row>
-    <row r="229" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D229" s="6"/>
+    <row r="231" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D231" s="6"/>
+      <c r="E231" s="4"/>
     </row>
     <row r="232" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E232" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="D232" s="6"/>
+      <c r="E232" s="4"/>
     </row>
     <row r="233" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D233" s="6"/>
     </row>
-    <row r="235" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E235" s="4" t="s">
+    <row r="236" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E236" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="237" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D237" s="6"/>
+    </row>
+    <row r="239" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E239" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="236" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D236" s="6"/>
-    </row>
-    <row r="238" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E238" s="4" t="s">
+    <row r="240" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D240" s="6"/>
+    </row>
+    <row r="242" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E242" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="239" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D239" s="6" t="s">
+    <row r="243" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D243" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E239" t="s">
+      <c r="E243" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="244" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E244" s="7" t="s">
+    <row r="248" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E248" s="7" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new db changes orbitposts
</commit_message>
<xml_diff>
--- a/FileGunBasin/9 August-04 StormBasin/230 next push hurricane/230 next push hurricane 1.xlsx
+++ b/FileGunBasin/9 August-04 StormBasin/230 next push hurricane/230 next push hurricane 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylecampbell/Documents/repos/localrepo-snefuru4/FileGunBasin/9 August-04 StormBasin/230 next push hurricane/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EE65B5-4FEF-B349-BF45-7AD7274942E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D67780-20E8-3649-93BB-A6CDFF47975F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19320" xr2:uid="{A19E904F-4B03-2145-9BA6-C366915416CF}"/>
   </bookViews>
@@ -768,8 +768,8 @@
   <dimension ref="D1:H248"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F146" sqref="F146"/>
+      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="E170" sqref="E170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>